<commit_message>
SKILIKS-3001. Reimport to 22.242 with 2013 year in mails.
</commit_message>
<xml_diff>
--- a/media/scenario_tutorial_22.242.xlsx
+++ b/media/scenario_tutorial_22.242.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr backupFile="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="21840" windowHeight="13680" tabRatio="938" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="21840" windowHeight="13680" tabRatio="938" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ALL DIALOGUES(E+T+RS+RV)" sheetId="37" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Mail!$A$2:$DC$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'to-do-list'!$A$1:$M$41</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -4596,7 +4596,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Ассистент </t>
@@ -4607,7 +4606,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t>Г</t>
@@ -4618,7 +4616,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t>енерального директора</t>
@@ -4631,7 +4628,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t>Н</t>
@@ -4642,7 +4638,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t>ач</t>
@@ -4653,7 +4648,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">альник </t>
@@ -4664,7 +4658,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">отдела </t>
@@ -4675,7 +4668,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t>информационных технологий (ИТ)</t>
@@ -5285,7 +5277,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t>службы</t>
@@ -5296,7 +5287,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> кадров</t>
@@ -6328,7 +6318,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10430,6 +10419,114 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="26" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="23" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="9" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="30" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="29" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="30" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="21" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="6" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="23" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="43" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="29" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="29" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="43" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="30" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="23" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="26" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="9" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="26" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="10" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="23" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="43" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="29" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="26" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="9" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="10" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="49" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="18" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="9" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="29" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -10469,112 +10566,73 @@
     <xf numFmtId="0" fontId="8" fillId="28" borderId="30" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="26" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="23" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="9" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="30" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="29" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="30" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="21" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="6" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="23" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="43" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="29" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="29" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="43" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="30" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="23" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="26" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="9" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="26" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="10" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="23" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="43" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="29" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="26" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="9" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="10" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="49" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="18" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="9" xfId="1217" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10653,75 +10711,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -12806,185 +12795,185 @@
       <selection pane="bottomRight" activeCell="DJ13" sqref="DJ13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="6.375" style="113" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="6.375" style="113" customWidth="1"/>
-    <col min="4" max="4" width="7.375" style="113" customWidth="1"/>
-    <col min="5" max="5" width="6.375" style="113" customWidth="1"/>
-    <col min="6" max="6" width="6.375" style="113" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.125" style="114" customWidth="1"/>
+    <col min="1" max="2" width="6.33203125" style="113" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="6.33203125" style="113" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="113" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="113" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="113" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.1640625" style="114" customWidth="1"/>
     <col min="8" max="8" width="32.5" style="115" customWidth="1"/>
-    <col min="9" max="9" width="6.625" style="116" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="116" customWidth="1"/>
     <col min="10" max="10" width="6.5" style="116" customWidth="1"/>
     <col min="11" max="11" width="6.5" style="116" customWidth="1" outlineLevel="1"/>
     <col min="12" max="12" width="11.5" style="110" customWidth="1"/>
     <col min="13" max="13" width="11.5" style="110" customWidth="1" outlineLevel="1"/>
     <col min="14" max="14" width="6.5" style="116" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="11.625" style="116" customWidth="1"/>
-    <col min="16" max="16" width="11.625" style="116" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="18" width="8.125" style="116" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="74.875" style="117" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="8.625" style="202" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="9.625" style="116" customWidth="1"/>
-    <col min="22" max="22" width="6.625" style="114" customWidth="1"/>
-    <col min="23" max="23" width="13.125" style="110" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="25" width="21.875" style="110" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="11.6640625" style="116" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="116" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="18" width="8.1640625" style="116" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="74.83203125" style="117" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="8.6640625" style="202" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="9.6640625" style="116" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" style="114" customWidth="1"/>
+    <col min="23" max="23" width="13.1640625" style="110" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="25" width="21.83203125" style="110" customWidth="1" outlineLevel="1"/>
     <col min="26" max="26" width="11" style="110" customWidth="1"/>
-    <col min="27" max="27" width="6.625" style="116" customWidth="1"/>
-    <col min="28" max="28" width="6.625" style="107" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="30" width="12.625" style="107" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="32" width="8.625" style="147" customWidth="1"/>
-    <col min="33" max="35" width="8.625" style="106" customWidth="1"/>
-    <col min="36" max="36" width="8.625" style="148" customWidth="1"/>
-    <col min="37" max="39" width="8.625" style="106" customWidth="1"/>
-    <col min="40" max="50" width="8.625" style="106" customWidth="1" outlineLevel="1"/>
-    <col min="51" max="51" width="8.625" style="106" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="52" max="52" width="17.125" style="106" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="55" width="8.625" style="148" customWidth="1"/>
-    <col min="56" max="57" width="8.625" style="106" customWidth="1"/>
-    <col min="58" max="58" width="8.625" style="148" customWidth="1"/>
-    <col min="59" max="61" width="8.625" style="106" customWidth="1"/>
-    <col min="62" max="63" width="8.625" style="148" customWidth="1"/>
-    <col min="64" max="66" width="8.625" style="106" customWidth="1"/>
-    <col min="67" max="68" width="8.625" style="106" customWidth="1" outlineLevel="1"/>
-    <col min="69" max="69" width="8.625" style="148" customWidth="1" outlineLevel="1"/>
-    <col min="70" max="70" width="8.625" style="106" customWidth="1" outlineLevel="1"/>
-    <col min="71" max="71" width="8.625" style="148" customWidth="1" outlineLevel="1"/>
-    <col min="72" max="74" width="8.625" style="106" customWidth="1" outlineLevel="1"/>
-    <col min="75" max="86" width="8.625" style="106" customWidth="1"/>
-    <col min="87" max="87" width="11.375" style="106" customWidth="1"/>
-    <col min="88" max="88" width="11.125" style="106" customWidth="1"/>
-    <col min="89" max="95" width="8.625" style="106" customWidth="1"/>
-    <col min="96" max="96" width="8.625" style="148" customWidth="1"/>
-    <col min="97" max="102" width="8.625" style="106" customWidth="1"/>
-    <col min="103" max="104" width="6.375" style="113" customWidth="1"/>
+    <col min="27" max="27" width="6.6640625" style="116" customWidth="1"/>
+    <col min="28" max="28" width="6.6640625" style="107" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="30" width="12.6640625" style="107" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="32" width="8.6640625" style="147" customWidth="1"/>
+    <col min="33" max="35" width="8.6640625" style="106" customWidth="1"/>
+    <col min="36" max="36" width="8.6640625" style="148" customWidth="1"/>
+    <col min="37" max="39" width="8.6640625" style="106" customWidth="1"/>
+    <col min="40" max="50" width="8.6640625" style="106" customWidth="1" outlineLevel="1"/>
+    <col min="51" max="51" width="8.6640625" style="106" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="52" max="52" width="17.1640625" style="106" customWidth="1" outlineLevel="1"/>
+    <col min="53" max="55" width="8.6640625" style="148" customWidth="1"/>
+    <col min="56" max="57" width="8.6640625" style="106" customWidth="1"/>
+    <col min="58" max="58" width="8.6640625" style="148" customWidth="1"/>
+    <col min="59" max="61" width="8.6640625" style="106" customWidth="1"/>
+    <col min="62" max="63" width="8.6640625" style="148" customWidth="1"/>
+    <col min="64" max="66" width="8.6640625" style="106" customWidth="1"/>
+    <col min="67" max="68" width="8.6640625" style="106" customWidth="1" outlineLevel="1"/>
+    <col min="69" max="69" width="8.6640625" style="148" customWidth="1" outlineLevel="1"/>
+    <col min="70" max="70" width="8.6640625" style="106" customWidth="1" outlineLevel="1"/>
+    <col min="71" max="71" width="8.6640625" style="148" customWidth="1" outlineLevel="1"/>
+    <col min="72" max="74" width="8.6640625" style="106" customWidth="1" outlineLevel="1"/>
+    <col min="75" max="86" width="8.6640625" style="106" customWidth="1"/>
+    <col min="87" max="87" width="11.33203125" style="106" customWidth="1"/>
+    <col min="88" max="88" width="11.1640625" style="106" customWidth="1"/>
+    <col min="89" max="95" width="8.6640625" style="106" customWidth="1"/>
+    <col min="96" max="96" width="8.6640625" style="148" customWidth="1"/>
+    <col min="97" max="102" width="8.6640625" style="106" customWidth="1"/>
+    <col min="103" max="104" width="6.33203125" style="113" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:104" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:104" ht="59.25" customHeight="1" thickBot="1">
       <c r="AB1" s="116"/>
       <c r="AC1" s="116"/>
       <c r="AD1" s="116"/>
-      <c r="AE1" s="386" t="s">
+      <c r="AE1" s="373" t="s">
         <v>100</v>
       </c>
-      <c r="AF1" s="387"/>
-      <c r="AG1" s="393" t="s">
+      <c r="AF1" s="374"/>
+      <c r="AG1" s="380" t="s">
         <v>8</v>
       </c>
-      <c r="AH1" s="394"/>
-      <c r="AI1" s="394"/>
-      <c r="AJ1" s="394"/>
-      <c r="AK1" s="394"/>
-      <c r="AL1" s="395"/>
-      <c r="AM1" s="396"/>
-      <c r="AN1" s="397" t="s">
+      <c r="AH1" s="381"/>
+      <c r="AI1" s="381"/>
+      <c r="AJ1" s="381"/>
+      <c r="AK1" s="381"/>
+      <c r="AL1" s="382"/>
+      <c r="AM1" s="383"/>
+      <c r="AN1" s="384" t="s">
         <v>9</v>
       </c>
-      <c r="AO1" s="398"/>
-      <c r="AP1" s="398"/>
-      <c r="AQ1" s="399" t="s">
+      <c r="AO1" s="385"/>
+      <c r="AP1" s="385"/>
+      <c r="AQ1" s="386" t="s">
         <v>10</v>
       </c>
-      <c r="AR1" s="400"/>
-      <c r="AS1" s="400"/>
-      <c r="AT1" s="400"/>
-      <c r="AU1" s="400"/>
-      <c r="AV1" s="401"/>
-      <c r="AW1" s="401"/>
-      <c r="AX1" s="401"/>
-      <c r="AY1" s="384" t="s">
+      <c r="AR1" s="387"/>
+      <c r="AS1" s="387"/>
+      <c r="AT1" s="387"/>
+      <c r="AU1" s="387"/>
+      <c r="AV1" s="388"/>
+      <c r="AW1" s="388"/>
+      <c r="AX1" s="388"/>
+      <c r="AY1" s="371" t="s">
         <v>11</v>
       </c>
-      <c r="AZ1" s="385"/>
-      <c r="BA1" s="404" t="s">
+      <c r="AZ1" s="372"/>
+      <c r="BA1" s="391" t="s">
         <v>89</v>
       </c>
-      <c r="BB1" s="405"/>
-      <c r="BC1" s="406"/>
-      <c r="BD1" s="407" t="s">
+      <c r="BB1" s="392"/>
+      <c r="BC1" s="393"/>
+      <c r="BD1" s="394" t="s">
         <v>90</v>
       </c>
-      <c r="BE1" s="408"/>
-      <c r="BF1" s="409" t="s">
+      <c r="BE1" s="395"/>
+      <c r="BF1" s="396" t="s">
         <v>12</v>
       </c>
-      <c r="BG1" s="410"/>
-      <c r="BH1" s="411"/>
-      <c r="BI1" s="366" t="s">
+      <c r="BG1" s="397"/>
+      <c r="BH1" s="398"/>
+      <c r="BI1" s="402" t="s">
         <v>91</v>
       </c>
-      <c r="BJ1" s="367"/>
-      <c r="BK1" s="367"/>
-      <c r="BL1" s="368" t="s">
+      <c r="BJ1" s="403"/>
+      <c r="BK1" s="403"/>
+      <c r="BL1" s="404" t="s">
         <v>92</v>
       </c>
-      <c r="BM1" s="369"/>
-      <c r="BN1" s="369"/>
-      <c r="BO1" s="370" t="s">
+      <c r="BM1" s="405"/>
+      <c r="BN1" s="405"/>
+      <c r="BO1" s="406" t="s">
         <v>93</v>
       </c>
-      <c r="BP1" s="371"/>
-      <c r="BQ1" s="371"/>
-      <c r="BR1" s="371"/>
-      <c r="BS1" s="371"/>
-      <c r="BT1" s="372" t="s">
+      <c r="BP1" s="407"/>
+      <c r="BQ1" s="407"/>
+      <c r="BR1" s="407"/>
+      <c r="BS1" s="407"/>
+      <c r="BT1" s="408" t="s">
         <v>94</v>
       </c>
-      <c r="BU1" s="373"/>
-      <c r="BV1" s="374"/>
-      <c r="BW1" s="375" t="s">
+      <c r="BU1" s="409"/>
+      <c r="BV1" s="410"/>
+      <c r="BW1" s="411" t="s">
         <v>95</v>
       </c>
-      <c r="BX1" s="376"/>
-      <c r="BY1" s="376"/>
-      <c r="BZ1" s="377"/>
-      <c r="CA1" s="377"/>
-      <c r="CB1" s="377"/>
-      <c r="CC1" s="378"/>
-      <c r="CD1" s="412" t="s">
+      <c r="BX1" s="412"/>
+      <c r="BY1" s="412"/>
+      <c r="BZ1" s="413"/>
+      <c r="CA1" s="413"/>
+      <c r="CB1" s="413"/>
+      <c r="CC1" s="414"/>
+      <c r="CD1" s="399" t="s">
         <v>106</v>
       </c>
-      <c r="CE1" s="413"/>
-      <c r="CF1" s="402" t="s">
+      <c r="CE1" s="400"/>
+      <c r="CF1" s="389" t="s">
         <v>107</v>
       </c>
-      <c r="CG1" s="414"/>
-      <c r="CH1" s="403"/>
-      <c r="CI1" s="402" t="s">
+      <c r="CG1" s="401"/>
+      <c r="CH1" s="390"/>
+      <c r="CI1" s="389" t="s">
         <v>13</v>
       </c>
-      <c r="CJ1" s="403"/>
+      <c r="CJ1" s="390"/>
       <c r="CK1" s="341" t="s">
         <v>96</v>
       </c>
       <c r="CL1" s="118" t="s">
         <v>97</v>
       </c>
-      <c r="CM1" s="388" t="s">
+      <c r="CM1" s="375" t="s">
         <v>98</v>
       </c>
-      <c r="CN1" s="389"/>
-      <c r="CO1" s="390"/>
-      <c r="CP1" s="391" t="s">
+      <c r="CN1" s="376"/>
+      <c r="CO1" s="377"/>
+      <c r="CP1" s="378" t="s">
         <v>108</v>
       </c>
-      <c r="CQ1" s="392"/>
+      <c r="CQ1" s="379"/>
       <c r="CR1" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="CS1" s="379" t="s">
+      <c r="CS1" s="366" t="s">
         <v>110</v>
       </c>
-      <c r="CT1" s="380"/>
-      <c r="CU1" s="380"/>
-      <c r="CV1" s="381" t="s">
+      <c r="CT1" s="367"/>
+      <c r="CU1" s="367"/>
+      <c r="CV1" s="368" t="s">
         <v>111</v>
       </c>
-      <c r="CW1" s="382"/>
-      <c r="CX1" s="383"/>
+      <c r="CW1" s="369"/>
+      <c r="CX1" s="370"/>
     </row>
-    <row r="2" spans="1:104" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:104" ht="79.5" thickBot="1">
       <c r="A2" s="120" t="s">
         <v>213</v>
       </c>
@@ -13301,6 +13290,11 @@
   </sheetData>
   <autoFilter ref="A2:CY2"/>
   <mergeCells count="21">
+    <mergeCell ref="BI1:BK1"/>
+    <mergeCell ref="BL1:BN1"/>
+    <mergeCell ref="BO1:BS1"/>
+    <mergeCell ref="BT1:BV1"/>
+    <mergeCell ref="BW1:CC1"/>
     <mergeCell ref="CS1:CU1"/>
     <mergeCell ref="CV1:CX1"/>
     <mergeCell ref="AY1:AZ1"/>
@@ -13317,11 +13311,6 @@
     <mergeCell ref="BF1:BH1"/>
     <mergeCell ref="CD1:CE1"/>
     <mergeCell ref="CF1:CH1"/>
-    <mergeCell ref="BI1:BK1"/>
-    <mergeCell ref="BL1:BN1"/>
-    <mergeCell ref="BO1:BS1"/>
-    <mergeCell ref="BT1:BV1"/>
-    <mergeCell ref="BW1:CC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -13347,31 +13336,31 @@
       <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="53" customWidth="1"/>
-    <col min="2" max="2" width="44.625" style="57" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="53" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" style="57" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.875" style="53" customWidth="1"/>
-    <col min="6" max="6" width="9.375" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="57" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.375" customWidth="1"/>
-    <col min="9" max="9" width="20.125" customWidth="1"/>
+    <col min="4" max="5" width="12.83203125" style="53" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="57" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="13.5" customWidth="1"/>
-    <col min="12" max="12" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="15" width="16.875" customWidth="1"/>
+    <col min="14" max="15" width="16.83203125" customWidth="1"/>
     <col min="16" max="16" width="56.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="54.625" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="39.125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="12.125" style="53" customWidth="1"/>
-    <col min="21" max="21" width="44.625" style="57" customWidth="1"/>
+    <col min="17" max="17" width="54.6640625" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="39.1640625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" style="53" customWidth="1"/>
+    <col min="21" max="21" width="44.6640625" style="57" customWidth="1"/>
     <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.875" style="53" customWidth="1"/>
+    <col min="23" max="23" width="12.83203125" style="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="9" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="9" customFormat="1" ht="48" thickBot="1">
       <c r="A1" s="233" t="s">
         <v>566</v>
       </c>
@@ -13442,7 +13431,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="10" customFormat="1">
       <c r="A2" s="61">
         <v>1</v>
       </c>
@@ -13497,7 +13486,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="10" customFormat="1">
       <c r="A3" s="59">
         <v>2</v>
       </c>
@@ -13552,7 +13541,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="10" customFormat="1">
       <c r="A4" s="59">
         <v>3</v>
       </c>
@@ -13607,7 +13596,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="10" customFormat="1">
       <c r="A5" s="59">
         <v>4</v>
       </c>
@@ -13662,7 +13651,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" s="3" customFormat="1">
       <c r="A6" s="59">
         <v>43</v>
       </c>
@@ -13721,7 +13710,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" s="10" customFormat="1">
       <c r="A7" s="59">
         <v>53</v>
       </c>
@@ -13784,7 +13773,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" s="10" customFormat="1">
       <c r="A8" s="59">
         <v>54</v>
       </c>
@@ -13847,7 +13836,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="10" customFormat="1">
       <c r="A9" s="59">
         <v>54</v>
       </c>
@@ -13910,7 +13899,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" s="10" customFormat="1">
       <c r="A10" s="59">
         <v>55</v>
       </c>
@@ -13973,7 +13962,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" s="10" customFormat="1">
       <c r="A11" s="59">
         <v>92</v>
       </c>
@@ -14036,7 +14025,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" s="10" customFormat="1">
       <c r="A12" s="59">
         <v>92</v>
       </c>
@@ -14099,7 +14088,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" s="10" customFormat="1">
       <c r="A13" s="59">
         <v>61</v>
       </c>
@@ -14162,7 +14151,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" s="10" customFormat="1">
       <c r="A14" s="59">
         <v>62</v>
       </c>
@@ -14225,7 +14214,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" s="3" customFormat="1">
       <c r="A15" s="59">
         <v>66</v>
       </c>
@@ -14288,7 +14277,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" s="3" customFormat="1">
       <c r="A16" s="59">
         <v>67</v>
       </c>
@@ -14351,7 +14340,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" s="3" customFormat="1">
       <c r="A17" s="59">
         <v>69</v>
       </c>
@@ -14414,7 +14403,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" s="3" customFormat="1">
       <c r="A18" s="59">
         <v>70</v>
       </c>
@@ -14477,7 +14466,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" s="3" customFormat="1">
       <c r="A19" s="59">
         <v>70</v>
       </c>
@@ -14540,7 +14529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" s="3" customFormat="1">
       <c r="A20" s="59">
         <v>85</v>
       </c>
@@ -14603,7 +14592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" s="10" customFormat="1">
       <c r="A21" s="59">
         <v>93</v>
       </c>
@@ -14666,7 +14655,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" s="10" customFormat="1">
       <c r="A22" s="59">
         <v>94</v>
       </c>
@@ -14729,7 +14718,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" s="10" customFormat="1">
       <c r="A23" s="59">
         <v>95</v>
       </c>
@@ -14792,7 +14781,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" s="10" customFormat="1">
       <c r="A24" s="59">
         <v>96</v>
       </c>
@@ -14855,7 +14844,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" s="10" customFormat="1">
       <c r="A25" s="59">
         <v>97</v>
       </c>
@@ -14918,7 +14907,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" s="10" customFormat="1">
       <c r="A26" s="59">
         <v>99</v>
       </c>
@@ -14981,7 +14970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" s="10" customFormat="1">
       <c r="A27" s="59">
         <v>100</v>
       </c>
@@ -15044,7 +15033,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" s="10" customFormat="1">
       <c r="A28" s="59">
         <v>102</v>
       </c>
@@ -15107,7 +15096,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" s="10" customFormat="1">
       <c r="A29" s="59">
         <v>101</v>
       </c>
@@ -15170,7 +15159,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" s="10" customFormat="1">
       <c r="A30" s="59">
         <v>103</v>
       </c>
@@ -15233,7 +15222,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" s="10" customFormat="1">
       <c r="A31" s="59">
         <v>104</v>
       </c>
@@ -15296,7 +15285,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" s="10" customFormat="1">
       <c r="A32" s="59">
         <v>105</v>
       </c>
@@ -15359,7 +15348,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" s="10" customFormat="1">
       <c r="A33" s="59">
         <v>106</v>
       </c>
@@ -15422,7 +15411,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" s="10" customFormat="1">
       <c r="A34" s="59">
         <v>107</v>
       </c>
@@ -15485,7 +15474,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" s="10" customFormat="1">
       <c r="A35" s="59">
         <v>108</v>
       </c>
@@ -15548,7 +15537,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" s="10" customFormat="1">
       <c r="A36" s="59">
         <v>109</v>
       </c>
@@ -15611,7 +15600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" s="10" customFormat="1">
       <c r="A37" s="59">
         <v>110</v>
       </c>
@@ -15674,7 +15663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" s="10" customFormat="1">
       <c r="A38" s="59">
         <v>111</v>
       </c>
@@ -15737,7 +15726,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" s="10" customFormat="1">
       <c r="A39" s="59">
         <v>112</v>
       </c>
@@ -15800,7 +15789,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" s="10" customFormat="1">
       <c r="A40" s="59">
         <v>113</v>
       </c>
@@ -15863,7 +15852,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" s="10" customFormat="1">
       <c r="A41" s="59">
         <v>115</v>
       </c>
@@ -15926,7 +15915,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" s="10" customFormat="1">
       <c r="A42" s="59">
         <v>114</v>
       </c>
@@ -15989,7 +15978,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" s="10" customFormat="1">
       <c r="A43" s="59">
         <v>116</v>
       </c>
@@ -16052,7 +16041,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" s="10" customFormat="1">
       <c r="A44" s="59">
         <v>116</v>
       </c>
@@ -16115,7 +16104,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" s="10" customFormat="1">
       <c r="A45" s="59">
         <v>117</v>
       </c>
@@ -16178,7 +16167,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" s="10" customFormat="1">
       <c r="A46" s="59">
         <v>118</v>
       </c>
@@ -16241,7 +16230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" s="10" customFormat="1">
       <c r="A47" s="59">
         <v>119</v>
       </c>
@@ -16304,7 +16293,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" s="10" customFormat="1">
       <c r="A48" s="59">
         <v>120</v>
       </c>
@@ -16367,7 +16356,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" s="10" customFormat="1">
       <c r="A49" s="59">
         <v>121</v>
       </c>
@@ -16430,7 +16419,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" s="10" customFormat="1">
       <c r="A50" s="59">
         <v>122</v>
       </c>
@@ -16493,7 +16482,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" s="10" customFormat="1">
       <c r="A51" s="59">
         <v>124</v>
       </c>
@@ -16556,7 +16545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:23" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" s="10" customFormat="1" ht="31.5">
       <c r="A52" s="59">
         <v>123</v>
       </c>
@@ -16619,7 +16608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" s="10" customFormat="1">
       <c r="A53" s="59">
         <v>125</v>
       </c>
@@ -16682,7 +16671,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" s="10" customFormat="1">
       <c r="A54" s="59">
         <v>127</v>
       </c>
@@ -16745,7 +16734,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" s="10" customFormat="1">
       <c r="A55" s="59">
         <v>127</v>
       </c>
@@ -16808,7 +16797,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" s="10" customFormat="1">
       <c r="A56" s="59">
         <v>127</v>
       </c>
@@ -16871,7 +16860,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" s="10" customFormat="1">
       <c r="A57" s="59">
         <v>127</v>
       </c>
@@ -16934,7 +16923,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" s="10" customFormat="1">
       <c r="A58" s="59">
         <v>127</v>
       </c>
@@ -16997,7 +16986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" s="10" customFormat="1">
       <c r="A59" s="59">
         <v>127</v>
       </c>
@@ -17060,7 +17049,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" s="10" customFormat="1">
       <c r="A60" s="59">
         <v>127</v>
       </c>
@@ -17123,7 +17112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" s="10" customFormat="1">
       <c r="A61" s="59">
         <v>127</v>
       </c>
@@ -17186,7 +17175,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" s="10" customFormat="1">
       <c r="A62" s="59">
         <v>127</v>
       </c>
@@ -17249,7 +17238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" s="10" customFormat="1">
       <c r="A63" s="59">
         <v>127</v>
       </c>
@@ -17312,7 +17301,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" s="10" customFormat="1">
       <c r="A64" s="59">
         <v>127</v>
       </c>
@@ -17375,7 +17364,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" s="10" customFormat="1">
       <c r="A65" s="59">
         <v>127</v>
       </c>
@@ -17438,7 +17427,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" s="10" customFormat="1">
       <c r="A66" s="59">
         <v>127</v>
       </c>
@@ -17501,7 +17490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" s="10" customFormat="1">
       <c r="A67" s="59">
         <v>127</v>
       </c>
@@ -17564,7 +17553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" s="10" customFormat="1">
       <c r="A68" s="59">
         <v>127</v>
       </c>
@@ -17627,7 +17616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" s="10" customFormat="1">
       <c r="A69" s="59">
         <v>127</v>
       </c>
@@ -17690,7 +17679,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" s="10" customFormat="1">
       <c r="A70" s="59">
         <v>127</v>
       </c>
@@ -17753,7 +17742,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" s="10" customFormat="1">
       <c r="A71" s="59">
         <v>127</v>
       </c>
@@ -17816,7 +17805,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" s="10" customFormat="1">
       <c r="A72" s="59">
         <v>127</v>
       </c>
@@ -17879,7 +17868,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:23" s="10" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:23" s="10" customFormat="1" ht="16.5" thickBot="1">
       <c r="A73" s="60">
         <v>127</v>
       </c>
@@ -17963,202 +17952,202 @@
   </sheetPr>
   <dimension ref="A1:DC7"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane xSplit="12" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F23" sqref="F23"/>
       <selection pane="topRight" activeCell="F23" sqref="F23"/>
       <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="11.375" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="8.875" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="5.875" style="8" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="14.625" style="15" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="7.125" style="15" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="12.875" style="15" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="8.125" style="15" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="7.875" style="15" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="11" width="8.125" style="15" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="13.625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="8.83203125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="5.83203125" style="8" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="14.6640625" style="15" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="7.1640625" style="15" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="12.83203125" style="15" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="8.1640625" style="15" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="7.83203125" style="15" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="11" width="8.1640625" style="15" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="13.6640625" style="15" customWidth="1"/>
     <col min="13" max="13" width="66.5" style="1" customWidth="1"/>
-    <col min="14" max="16" width="10.125" style="15" customWidth="1"/>
+    <col min="14" max="16" width="10.1640625" style="15" customWidth="1"/>
     <col min="17" max="17" width="8" style="15" customWidth="1"/>
-    <col min="18" max="21" width="10.125" style="15" customWidth="1"/>
+    <col min="18" max="21" width="10.1640625" style="15" customWidth="1"/>
     <col min="22" max="22" width="8" style="15" customWidth="1"/>
-    <col min="23" max="23" width="11.625" style="8" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" style="8" customWidth="1"/>
     <col min="24" max="24" width="14" style="25" customWidth="1"/>
-    <col min="25" max="25" width="14.625" style="2" customWidth="1"/>
-    <col min="26" max="26" width="11.625" style="53" customWidth="1"/>
+    <col min="25" max="25" width="14.6640625" style="2" customWidth="1"/>
+    <col min="26" max="26" width="11.6640625" style="53" customWidth="1"/>
     <col min="27" max="27" width="20.5" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="29" width="8.625" style="6" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="32" width="8.625" customWidth="1"/>
-    <col min="33" max="33" width="8.625" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="36" width="8.625" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="8.625" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="38" max="47" width="8.625" customWidth="1" outlineLevel="1"/>
-    <col min="48" max="48" width="8.625" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="49" max="49" width="9.625" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="52" width="8.625" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="54" width="8.625" customWidth="1"/>
-    <col min="55" max="55" width="8.625" style="7" customWidth="1"/>
-    <col min="56" max="57" width="8.625" customWidth="1"/>
-    <col min="58" max="58" width="8.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="60" width="8.625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="61" max="65" width="8.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="8.625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="67" max="67" width="8.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="8.625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="69" max="71" width="8.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="72" max="72" width="8.625" customWidth="1" collapsed="1"/>
-    <col min="73" max="78" width="8.625" customWidth="1"/>
-    <col min="79" max="82" width="8.625" customWidth="1" outlineLevel="1"/>
-    <col min="83" max="83" width="8.625" customWidth="1"/>
-    <col min="84" max="84" width="11.375" customWidth="1"/>
-    <col min="85" max="85" width="11.125" customWidth="1"/>
-    <col min="86" max="86" width="8.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="8.625" customWidth="1" collapsed="1"/>
-    <col min="88" max="92" width="8.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="93" max="93" width="8.625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="94" max="94" width="8.625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="95" max="95" width="8.625" customWidth="1" collapsed="1"/>
-    <col min="96" max="99" width="8.625" customWidth="1"/>
-    <col min="101" max="101" width="35.625" customWidth="1"/>
-    <col min="103" max="103" width="13.875" style="1" customWidth="1"/>
-    <col min="104" max="104" width="12.25" style="1" customWidth="1"/>
+    <col min="28" max="29" width="8.6640625" style="6" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="32" width="8.6640625" customWidth="1"/>
+    <col min="33" max="33" width="8.6640625" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="36" width="8.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="8.6640625" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="38" max="47" width="8.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="48" max="48" width="8.6640625" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="49" max="49" width="9.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="52" width="8.6640625" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="53" max="54" width="8.6640625" customWidth="1"/>
+    <col min="55" max="55" width="8.6640625" style="7" customWidth="1"/>
+    <col min="56" max="57" width="8.6640625" customWidth="1"/>
+    <col min="58" max="58" width="8.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="60" width="8.6640625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="61" max="65" width="8.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="8.6640625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="67" max="67" width="8.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="68" max="68" width="8.6640625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="69" max="71" width="8.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="72" max="72" width="8.6640625" customWidth="1" collapsed="1"/>
+    <col min="73" max="78" width="8.6640625" customWidth="1"/>
+    <col min="79" max="82" width="8.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="83" max="83" width="8.6640625" customWidth="1"/>
+    <col min="84" max="84" width="11.33203125" customWidth="1"/>
+    <col min="85" max="85" width="11.1640625" customWidth="1"/>
+    <col min="86" max="86" width="8.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="87" max="87" width="8.6640625" customWidth="1" collapsed="1"/>
+    <col min="88" max="92" width="8.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="93" max="93" width="8.6640625" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="94" max="94" width="8.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="95" max="95" width="8.6640625" customWidth="1" collapsed="1"/>
+    <col min="96" max="99" width="8.6640625" customWidth="1"/>
+    <col min="101" max="101" width="35.6640625" customWidth="1"/>
+    <col min="103" max="103" width="13.83203125" style="1" customWidth="1"/>
+    <col min="104" max="104" width="12.1640625" style="1" customWidth="1"/>
     <col min="106" max="106" width="15" customWidth="1"/>
     <col min="107" max="107" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:107" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:107" ht="95.25" customHeight="1" thickBot="1">
       <c r="V1" s="15" t="s">
         <v>16</v>
       </c>
       <c r="Y1" s="53"/>
       <c r="AA1" s="53"/>
-      <c r="AB1" s="453" t="s">
+      <c r="AB1" s="415" t="s">
         <v>100</v>
       </c>
-      <c r="AC1" s="454"/>
-      <c r="AD1" s="455" t="s">
+      <c r="AC1" s="416"/>
+      <c r="AD1" s="417" t="s">
         <v>8</v>
       </c>
-      <c r="AE1" s="456"/>
-      <c r="AF1" s="456"/>
-      <c r="AG1" s="456"/>
-      <c r="AH1" s="456"/>
-      <c r="AI1" s="457"/>
-      <c r="AJ1" s="458"/>
-      <c r="AK1" s="459" t="s">
+      <c r="AE1" s="418"/>
+      <c r="AF1" s="418"/>
+      <c r="AG1" s="418"/>
+      <c r="AH1" s="418"/>
+      <c r="AI1" s="419"/>
+      <c r="AJ1" s="420"/>
+      <c r="AK1" s="421" t="s">
         <v>9</v>
       </c>
-      <c r="AL1" s="460"/>
-      <c r="AM1" s="460"/>
-      <c r="AN1" s="461" t="s">
+      <c r="AL1" s="422"/>
+      <c r="AM1" s="422"/>
+      <c r="AN1" s="423" t="s">
         <v>10</v>
       </c>
-      <c r="AO1" s="462"/>
-      <c r="AP1" s="462"/>
-      <c r="AQ1" s="462"/>
-      <c r="AR1" s="462"/>
-      <c r="AS1" s="463"/>
-      <c r="AT1" s="463"/>
-      <c r="AU1" s="463"/>
-      <c r="AV1" s="441" t="s">
+      <c r="AO1" s="424"/>
+      <c r="AP1" s="424"/>
+      <c r="AQ1" s="424"/>
+      <c r="AR1" s="424"/>
+      <c r="AS1" s="425"/>
+      <c r="AT1" s="425"/>
+      <c r="AU1" s="425"/>
+      <c r="AV1" s="426" t="s">
         <v>11</v>
       </c>
-      <c r="AW1" s="442"/>
-      <c r="AX1" s="443" t="s">
+      <c r="AW1" s="427"/>
+      <c r="AX1" s="428" t="s">
         <v>89</v>
       </c>
-      <c r="AY1" s="444"/>
-      <c r="AZ1" s="445"/>
-      <c r="BA1" s="446" t="s">
+      <c r="AY1" s="429"/>
+      <c r="AZ1" s="430"/>
+      <c r="BA1" s="431" t="s">
         <v>90</v>
       </c>
-      <c r="BB1" s="447"/>
-      <c r="BC1" s="448" t="s">
+      <c r="BB1" s="432"/>
+      <c r="BC1" s="433" t="s">
         <v>12</v>
       </c>
-      <c r="BD1" s="449"/>
-      <c r="BE1" s="450"/>
-      <c r="BF1" s="451" t="s">
+      <c r="BD1" s="434"/>
+      <c r="BE1" s="435"/>
+      <c r="BF1" s="436" t="s">
         <v>91</v>
       </c>
-      <c r="BG1" s="452"/>
-      <c r="BH1" s="452"/>
-      <c r="BI1" s="415" t="s">
+      <c r="BG1" s="437"/>
+      <c r="BH1" s="437"/>
+      <c r="BI1" s="438" t="s">
         <v>92</v>
       </c>
-      <c r="BJ1" s="416"/>
-      <c r="BK1" s="416"/>
-      <c r="BL1" s="417" t="s">
+      <c r="BJ1" s="439"/>
+      <c r="BK1" s="439"/>
+      <c r="BL1" s="440" t="s">
         <v>93</v>
       </c>
-      <c r="BM1" s="418"/>
-      <c r="BN1" s="418"/>
-      <c r="BO1" s="418"/>
-      <c r="BP1" s="418"/>
-      <c r="BQ1" s="419" t="s">
+      <c r="BM1" s="441"/>
+      <c r="BN1" s="441"/>
+      <c r="BO1" s="441"/>
+      <c r="BP1" s="441"/>
+      <c r="BQ1" s="442" t="s">
         <v>94</v>
       </c>
-      <c r="BR1" s="420"/>
-      <c r="BS1" s="421"/>
-      <c r="BT1" s="422" t="s">
+      <c r="BR1" s="443"/>
+      <c r="BS1" s="444"/>
+      <c r="BT1" s="445" t="s">
         <v>95</v>
       </c>
-      <c r="BU1" s="423"/>
-      <c r="BV1" s="423"/>
-      <c r="BW1" s="424"/>
-      <c r="BX1" s="424"/>
-      <c r="BY1" s="424"/>
-      <c r="BZ1" s="425"/>
-      <c r="CA1" s="429" t="s">
+      <c r="BU1" s="446"/>
+      <c r="BV1" s="446"/>
+      <c r="BW1" s="447"/>
+      <c r="BX1" s="447"/>
+      <c r="BY1" s="447"/>
+      <c r="BZ1" s="448"/>
+      <c r="CA1" s="452" t="s">
         <v>106</v>
       </c>
-      <c r="CB1" s="430"/>
-      <c r="CC1" s="436" t="s">
+      <c r="CB1" s="453"/>
+      <c r="CC1" s="459" t="s">
         <v>107</v>
       </c>
-      <c r="CD1" s="437"/>
-      <c r="CE1" s="438"/>
-      <c r="CF1" s="436" t="s">
+      <c r="CD1" s="460"/>
+      <c r="CE1" s="461"/>
+      <c r="CF1" s="459" t="s">
         <v>13</v>
       </c>
-      <c r="CG1" s="437"/>
+      <c r="CG1" s="460"/>
       <c r="CH1" s="342" t="s">
         <v>96</v>
       </c>
       <c r="CI1" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="CJ1" s="431" t="s">
+      <c r="CJ1" s="454" t="s">
         <v>98</v>
       </c>
-      <c r="CK1" s="432"/>
-      <c r="CL1" s="433"/>
-      <c r="CM1" s="439" t="s">
+      <c r="CK1" s="455"/>
+      <c r="CL1" s="456"/>
+      <c r="CM1" s="462" t="s">
         <v>108</v>
       </c>
-      <c r="CN1" s="440"/>
+      <c r="CN1" s="463"/>
       <c r="CO1" s="75" t="s">
         <v>109</v>
       </c>
-      <c r="CP1" s="434" t="s">
+      <c r="CP1" s="457" t="s">
         <v>110</v>
       </c>
-      <c r="CQ1" s="435"/>
-      <c r="CR1" s="435"/>
-      <c r="CS1" s="426" t="s">
+      <c r="CQ1" s="458"/>
+      <c r="CR1" s="458"/>
+      <c r="CS1" s="449" t="s">
         <v>111</v>
       </c>
-      <c r="CT1" s="427"/>
-      <c r="CU1" s="428"/>
+      <c r="CT1" s="450"/>
+      <c r="CU1" s="451"/>
     </row>
-    <row r="2" spans="1:107" s="17" customFormat="1" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:107" s="17" customFormat="1" ht="79.5" thickBot="1">
       <c r="A2" s="27" t="s">
         <v>573</v>
       </c>
@@ -18481,12 +18470,12 @@
         <v>628</v>
       </c>
     </row>
-    <row r="3" spans="1:107" s="3" customFormat="1" ht="142.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:107" s="3" customFormat="1" ht="142.5" thickBot="1">
       <c r="A3" s="299" t="s">
         <v>252</v>
       </c>
       <c r="B3" s="300">
-        <v>41185</v>
+        <v>41550</v>
       </c>
       <c r="C3" s="301">
         <v>0.43888888888888888</v>
@@ -18642,12 +18631,12 @@
         <v>798</v>
       </c>
     </row>
-    <row r="4" spans="1:107" s="3" customFormat="1" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:107" s="3" customFormat="1" ht="220.5">
       <c r="A4" s="317" t="s">
         <v>253</v>
       </c>
       <c r="B4" s="318">
-        <v>41185</v>
+        <v>41550</v>
       </c>
       <c r="C4" s="319">
         <v>0.4597222222222222</v>
@@ -18803,12 +18792,12 @@
         <v>798</v>
       </c>
     </row>
-    <row r="5" spans="1:107" s="3" customFormat="1" ht="158.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:107" s="3" customFormat="1" ht="158.25" thickBot="1">
       <c r="A5" s="85" t="s">
         <v>254</v>
       </c>
       <c r="B5" s="86">
-        <v>41180</v>
+        <v>41545</v>
       </c>
       <c r="C5" s="87">
         <v>0.78125</v>
@@ -18964,12 +18953,12 @@
         <v>798</v>
       </c>
     </row>
-    <row r="6" spans="1:107" s="3" customFormat="1" ht="142.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:107" s="3" customFormat="1" ht="142.5" thickBot="1">
       <c r="A6" s="334" t="s">
         <v>255</v>
       </c>
       <c r="B6" s="93">
-        <v>41183</v>
+        <v>41548</v>
       </c>
       <c r="C6" s="335">
         <v>0.6875</v>
@@ -19125,12 +19114,12 @@
         <v>798</v>
       </c>
     </row>
-    <row r="7" spans="1:107" s="3" customFormat="1" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:107" s="3" customFormat="1" ht="126.75" thickBot="1">
       <c r="A7" s="98" t="s">
         <v>251</v>
       </c>
       <c r="B7" s="99">
-        <v>41185</v>
+        <v>41550</v>
       </c>
       <c r="C7" s="100">
         <v>0.68055555555555547</v>
@@ -19291,16 +19280,6 @@
   </sheetData>
   <autoFilter ref="A2:DC7"/>
   <mergeCells count="21">
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AJ1"/>
-    <mergeCell ref="AK1:AM1"/>
-    <mergeCell ref="AN1:AR1"/>
-    <mergeCell ref="AS1:AU1"/>
-    <mergeCell ref="AV1:AW1"/>
-    <mergeCell ref="AX1:AZ1"/>
-    <mergeCell ref="BA1:BB1"/>
-    <mergeCell ref="BC1:BE1"/>
-    <mergeCell ref="BF1:BH1"/>
     <mergeCell ref="BI1:BK1"/>
     <mergeCell ref="BL1:BP1"/>
     <mergeCell ref="BQ1:BS1"/>
@@ -19312,6 +19291,16 @@
     <mergeCell ref="CC1:CE1"/>
     <mergeCell ref="CF1:CG1"/>
     <mergeCell ref="CM1:CN1"/>
+    <mergeCell ref="AV1:AW1"/>
+    <mergeCell ref="AX1:AZ1"/>
+    <mergeCell ref="BA1:BB1"/>
+    <mergeCell ref="BC1:BE1"/>
+    <mergeCell ref="BF1:BH1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AJ1"/>
+    <mergeCell ref="AK1:AM1"/>
+    <mergeCell ref="AN1:AR1"/>
+    <mergeCell ref="AS1:AU1"/>
   </mergeCells>
   <conditionalFormatting sqref="DC3:DC7">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -19331,28 +19320,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="53" customWidth="1"/>
-    <col min="2" max="2" width="8.625" style="53" customWidth="1"/>
-    <col min="3" max="3" width="45.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.625" style="53" customWidth="1"/>
-    <col min="6" max="10" width="7.625" style="53" customWidth="1"/>
-    <col min="11" max="11" width="63.125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.875" customWidth="1"/>
-    <col min="13" max="13" width="14.375" style="53" customWidth="1"/>
-    <col min="14" max="14" width="32.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="53" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="53" customWidth="1"/>
+    <col min="3" max="3" width="45.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="53" customWidth="1"/>
+    <col min="6" max="10" width="7.6640625" style="53" customWidth="1"/>
+    <col min="11" max="11" width="63.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.83203125" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" style="53" customWidth="1"/>
+    <col min="14" max="14" width="32.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="32.25" thickBot="1">
       <c r="A1" s="214" t="s">
         <v>586</v>
       </c>
@@ -19396,7 +19385,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="10" customFormat="1" ht="31.5">
       <c r="A2" s="197" t="s">
         <v>264</v>
       </c>
@@ -19438,7 +19427,7 @@
       </c>
       <c r="N2" s="73"/>
     </row>
-    <row r="3" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="10" customFormat="1">
       <c r="A3" s="198" t="s">
         <v>236</v>
       </c>
@@ -19476,7 +19465,7 @@
       </c>
       <c r="N3" s="65"/>
     </row>
-    <row r="4" spans="1:14" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="10" customFormat="1" ht="47.25">
       <c r="A4" s="198" t="s">
         <v>265</v>
       </c>
@@ -19518,7 +19507,7 @@
       </c>
       <c r="N4" s="65"/>
     </row>
-    <row r="5" spans="1:14" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="10" customFormat="1" ht="31.5">
       <c r="A5" s="198" t="s">
         <v>266</v>
       </c>
@@ -19556,7 +19545,7 @@
       </c>
       <c r="N5" s="65"/>
     </row>
-    <row r="6" spans="1:14" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="10" customFormat="1" ht="31.5">
       <c r="A6" s="198" t="s">
         <v>240</v>
       </c>
@@ -19598,7 +19587,7 @@
       </c>
       <c r="N6" s="65"/>
     </row>
-    <row r="7" spans="1:14" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="10" customFormat="1" ht="31.5">
       <c r="A7" s="198" t="s">
         <v>241</v>
       </c>
@@ -19640,7 +19629,7 @@
       </c>
       <c r="N7" s="65"/>
     </row>
-    <row r="8" spans="1:14" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="10" customFormat="1" ht="31.5">
       <c r="A8" s="198" t="s">
         <v>218</v>
       </c>
@@ -19676,7 +19665,7 @@
       <c r="M8" s="14"/>
       <c r="N8" s="65"/>
     </row>
-    <row r="9" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="10" customFormat="1">
       <c r="A9" s="198" t="s">
         <v>220</v>
       </c>
@@ -19712,7 +19701,7 @@
       <c r="M9" s="14"/>
       <c r="N9" s="65"/>
     </row>
-    <row r="10" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="10" customFormat="1">
       <c r="A10" s="198" t="s">
         <v>221</v>
       </c>
@@ -19748,7 +19737,7 @@
       <c r="M10" s="14"/>
       <c r="N10" s="65"/>
     </row>
-    <row r="11" spans="1:14" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="10" customFormat="1" ht="31.5">
       <c r="A11" s="198" t="s">
         <v>219</v>
       </c>
@@ -19788,7 +19777,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="10" customFormat="1" ht="47.25">
       <c r="A12" s="198" t="s">
         <v>232</v>
       </c>
@@ -19824,7 +19813,7 @@
       <c r="M12" s="14"/>
       <c r="N12" s="65"/>
     </row>
-    <row r="13" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="10" customFormat="1">
       <c r="A13" s="198" t="s">
         <v>267</v>
       </c>
@@ -19860,7 +19849,7 @@
       <c r="M13" s="14"/>
       <c r="N13" s="65"/>
     </row>
-    <row r="14" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="10" customFormat="1">
       <c r="A14" s="198" t="s">
         <v>235</v>
       </c>
@@ -19896,7 +19885,7 @@
       <c r="M14" s="14"/>
       <c r="N14" s="65"/>
     </row>
-    <row r="15" spans="1:14" s="10" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="10" customFormat="1" ht="63">
       <c r="A15" s="198" t="s">
         <v>31</v>
       </c>
@@ -19938,7 +19927,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="10" customFormat="1">
       <c r="A16" s="199" t="s">
         <v>263</v>
       </c>
@@ -19976,7 +19965,7 @@
       </c>
       <c r="N16" s="84"/>
     </row>
-    <row r="17" spans="1:14" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="10" customFormat="1" ht="47.25">
       <c r="A17" s="199" t="s">
         <v>269</v>
       </c>
@@ -20014,7 +20003,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="10" customFormat="1">
       <c r="A18" s="199" t="s">
         <v>153</v>
       </c>
@@ -20050,7 +20039,7 @@
       <c r="M18" s="50"/>
       <c r="N18" s="84"/>
     </row>
-    <row r="19" spans="1:14" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="10" customFormat="1" ht="31.5">
       <c r="A19" s="198" t="s">
         <v>270</v>
       </c>
@@ -20086,7 +20075,7 @@
       <c r="M19" s="14"/>
       <c r="N19" s="65"/>
     </row>
-    <row r="20" spans="1:14" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="10" customFormat="1" ht="31.5">
       <c r="A20" s="198" t="s">
         <v>271</v>
       </c>
@@ -20122,7 +20111,7 @@
       <c r="M20" s="14"/>
       <c r="N20" s="65"/>
     </row>
-    <row r="21" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="10" customFormat="1">
       <c r="A21" s="198" t="s">
         <v>272</v>
       </c>
@@ -20158,7 +20147,7 @@
       <c r="M21" s="14"/>
       <c r="N21" s="65"/>
     </row>
-    <row r="22" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="10" customFormat="1">
       <c r="A22" s="198" t="s">
         <v>273</v>
       </c>
@@ -20194,7 +20183,7 @@
       <c r="M22" s="14"/>
       <c r="N22" s="65"/>
     </row>
-    <row r="23" spans="1:14" s="10" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" s="10" customFormat="1" ht="33.75" customHeight="1" thickBot="1">
       <c r="A23" s="364" t="s">
         <v>274</v>
       </c>
@@ -20236,17 +20225,22 @@
   <autoFilter ref="A1:N23"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
@@ -20254,22 +20248,22 @@
       <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="5.5" style="53" customWidth="1"/>
-    <col min="3" max="3" width="58.875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="9.875" style="15" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="6.625" style="15" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="9.625" style="15" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="6.625" style="15" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="6.125" style="53" customWidth="1"/>
-    <col min="10" max="10" width="5.625" style="53" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="54.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="58.83203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="9.83203125" style="15" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="6.6640625" style="15" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="9.6640625" style="15" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="6.6640625" style="15" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="6.1640625" style="53" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" style="53" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="54.1640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="8" customFormat="1" ht="48" thickBot="1">
       <c r="A1" s="27" t="s">
         <v>593</v>
       </c>
@@ -20310,7 +20304,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A2" s="264" t="s">
         <v>433</v>
       </c>
@@ -20341,7 +20335,7 @@
       <c r="L2" s="22"/>
       <c r="M2" s="46"/>
     </row>
-    <row r="3" spans="1:13" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="10" customFormat="1" ht="47.25">
       <c r="A3" s="45" t="s">
         <v>434</v>
       </c>
@@ -20378,7 +20372,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A4" s="45" t="s">
         <v>435</v>
       </c>
@@ -20415,7 +20409,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A5" s="45" t="s">
         <v>436</v>
       </c>
@@ -20452,7 +20446,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="10" customFormat="1">
       <c r="A6" s="45" t="s">
         <v>437</v>
       </c>
@@ -20483,7 +20477,7 @@
       <c r="L6" s="19"/>
       <c r="M6" s="47"/>
     </row>
-    <row r="7" spans="1:13" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="10" customFormat="1" ht="47.25">
       <c r="A7" s="45" t="s">
         <v>438</v>
       </c>
@@ -20516,7 +20510,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="10" customFormat="1">
       <c r="A8" s="45" t="s">
         <v>439</v>
       </c>
@@ -20553,7 +20547,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="10" customFormat="1">
       <c r="A9" s="45" t="s">
         <v>440</v>
       </c>
@@ -20582,7 +20576,7 @@
       <c r="L9" s="67"/>
       <c r="M9" s="47"/>
     </row>
-    <row r="10" spans="1:13" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="10" customFormat="1" ht="47.25">
       <c r="A10" s="45" t="s">
         <v>441</v>
       </c>
@@ -20617,7 +20611,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="10" customFormat="1">
       <c r="A11" s="45" t="s">
         <v>442</v>
       </c>
@@ -20650,7 +20644,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="10" customFormat="1" ht="78.75">
       <c r="A12" s="45" t="s">
         <v>443</v>
       </c>
@@ -20683,7 +20677,7 @@
       </c>
       <c r="M12" s="47"/>
     </row>
-    <row r="13" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A13" s="45" t="s">
         <v>444</v>
       </c>
@@ -20716,7 +20710,7 @@
       </c>
       <c r="M13" s="47"/>
     </row>
-    <row r="14" spans="1:13" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="10" customFormat="1" ht="47.25">
       <c r="A14" s="45" t="s">
         <v>445</v>
       </c>
@@ -20747,7 +20741,7 @@
       <c r="L14" s="19"/>
       <c r="M14" s="47"/>
     </row>
-    <row r="15" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A15" s="45" t="s">
         <v>30</v>
       </c>
@@ -20782,7 +20776,7 @@
       <c r="L15" s="19"/>
       <c r="M15" s="47"/>
     </row>
-    <row r="16" spans="1:13" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="10" customFormat="1" ht="47.25">
       <c r="A16" s="45" t="s">
         <v>446</v>
       </c>
@@ -20817,7 +20811,7 @@
       </c>
       <c r="M16" s="47"/>
     </row>
-    <row r="17" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="10" customFormat="1">
       <c r="A17" s="45" t="s">
         <v>447</v>
       </c>
@@ -20852,7 +20846,7 @@
       </c>
       <c r="M17" s="47"/>
     </row>
-    <row r="18" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A18" s="45" t="s">
         <v>448</v>
       </c>
@@ -20887,7 +20881,7 @@
       </c>
       <c r="M18" s="47"/>
     </row>
-    <row r="19" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="10" customFormat="1">
       <c r="A19" s="45" t="s">
         <v>449</v>
       </c>
@@ -20916,7 +20910,7 @@
       <c r="L19" s="19"/>
       <c r="M19" s="47"/>
     </row>
-    <row r="20" spans="1:13" s="10" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" s="10" customFormat="1" ht="16.5" thickBot="1">
       <c r="A20" s="45" t="s">
         <v>450</v>
       </c>
@@ -20949,7 +20943,7 @@
       <c r="L20" s="267"/>
       <c r="M20" s="265"/>
     </row>
-    <row r="21" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="10" customFormat="1">
       <c r="A21" s="264" t="s">
         <v>35</v>
       </c>
@@ -20982,7 +20976,7 @@
       <c r="L21" s="22"/>
       <c r="M21" s="46"/>
     </row>
-    <row r="22" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A22" s="45" t="s">
         <v>36</v>
       </c>
@@ -21011,7 +21005,7 @@
       <c r="L22" s="19"/>
       <c r="M22" s="47"/>
     </row>
-    <row r="23" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="10" customFormat="1">
       <c r="A23" s="45" t="s">
         <v>32</v>
       </c>
@@ -21040,7 +21034,7 @@
       <c r="L23" s="19"/>
       <c r="M23" s="47"/>
     </row>
-    <row r="24" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A24" s="45" t="s">
         <v>33</v>
       </c>
@@ -21069,7 +21063,7 @@
       <c r="L24" s="19"/>
       <c r="M24" s="47"/>
     </row>
-    <row r="25" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="10" customFormat="1">
       <c r="A25" s="45" t="s">
         <v>34</v>
       </c>
@@ -21098,7 +21092,7 @@
       <c r="L25" s="19"/>
       <c r="M25" s="47"/>
     </row>
-    <row r="26" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="10" customFormat="1">
       <c r="A26" s="45" t="s">
         <v>230</v>
       </c>
@@ -21127,7 +21121,7 @@
       <c r="L26" s="19"/>
       <c r="M26" s="47"/>
     </row>
-    <row r="27" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A27" s="45" t="s">
         <v>233</v>
       </c>
@@ -21156,7 +21150,7 @@
       <c r="L27" s="19"/>
       <c r="M27" s="47"/>
     </row>
-    <row r="28" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A28" s="45" t="s">
         <v>113</v>
       </c>
@@ -21185,7 +21179,7 @@
       <c r="L28" s="19"/>
       <c r="M28" s="47"/>
     </row>
-    <row r="29" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A29" s="45" t="s">
         <v>112</v>
       </c>
@@ -21218,7 +21212,7 @@
       <c r="L29" s="19"/>
       <c r="M29" s="47"/>
     </row>
-    <row r="30" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="10" customFormat="1">
       <c r="A30" s="45" t="s">
         <v>114</v>
       </c>
@@ -21247,7 +21241,7 @@
       <c r="L30" s="19"/>
       <c r="M30" s="47"/>
     </row>
-    <row r="31" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="10" customFormat="1">
       <c r="A31" s="45" t="s">
         <v>149</v>
       </c>
@@ -21280,7 +21274,7 @@
       <c r="L31" s="19"/>
       <c r="M31" s="47"/>
     </row>
-    <row r="32" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="10" customFormat="1">
       <c r="A32" s="45" t="s">
         <v>244</v>
       </c>
@@ -21309,7 +21303,7 @@
       <c r="L32" s="19"/>
       <c r="M32" s="47"/>
     </row>
-    <row r="33" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="10" customFormat="1">
       <c r="A33" s="45" t="s">
         <v>150</v>
       </c>
@@ -21338,7 +21332,7 @@
       <c r="L33" s="19"/>
       <c r="M33" s="47"/>
     </row>
-    <row r="34" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A34" s="45" t="s">
         <v>151</v>
       </c>
@@ -21367,7 +21361,7 @@
       <c r="L34" s="19"/>
       <c r="M34" s="47"/>
     </row>
-    <row r="35" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A35" s="268" t="s">
         <v>248</v>
       </c>
@@ -21396,7 +21390,7 @@
       <c r="L35" s="19"/>
       <c r="M35" s="47"/>
     </row>
-    <row r="36" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A36" s="269" t="s">
         <v>281</v>
       </c>
@@ -21427,7 +21421,7 @@
       <c r="L36" s="19"/>
       <c r="M36" s="47"/>
     </row>
-    <row r="37" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A37" s="269" t="s">
         <v>282</v>
       </c>
@@ -21458,7 +21452,7 @@
       <c r="L37" s="19"/>
       <c r="M37" s="47"/>
     </row>
-    <row r="38" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" s="10" customFormat="1" ht="31.5">
       <c r="A38" s="269" t="s">
         <v>283</v>
       </c>
@@ -21489,7 +21483,7 @@
       <c r="L38" s="19"/>
       <c r="M38" s="47"/>
     </row>
-    <row r="39" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="10" customFormat="1">
       <c r="A39" s="269" t="s">
         <v>284</v>
       </c>
@@ -21520,7 +21514,7 @@
       <c r="L39" s="19"/>
       <c r="M39" s="47"/>
     </row>
-    <row r="40" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" s="10" customFormat="1">
       <c r="A40" s="343" t="s">
         <v>285</v>
       </c>
@@ -21551,7 +21545,7 @@
       <c r="L40" s="348"/>
       <c r="M40" s="48"/>
     </row>
-    <row r="41" spans="1:13" s="10" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" s="10" customFormat="1" ht="32.25" thickBot="1">
       <c r="A41" s="270" t="s">
         <v>619</v>
       </c>
@@ -21580,7 +21574,7 @@
       <c r="L41" s="267"/>
       <c r="M41" s="265"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13">
       <c r="C42"/>
       <c r="D42" s="53"/>
       <c r="E42" s="53"/>
@@ -21588,7 +21582,7 @@
       <c r="G42" s="53"/>
       <c r="H42" s="53"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13">
       <c r="C43"/>
       <c r="D43" s="53"/>
       <c r="E43" s="53"/>
@@ -21596,7 +21590,7 @@
       <c r="G43" s="53"/>
       <c r="H43" s="53"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13">
       <c r="C45"/>
       <c r="D45" s="53"/>
       <c r="E45" s="53"/>
@@ -21604,7 +21598,7 @@
       <c r="G45" s="53"/>
       <c r="H45" s="53"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="C46"/>
       <c r="D46" s="53"/>
       <c r="E46" s="53"/>
@@ -21616,12 +21610,17 @@
   <autoFilter ref="A1:M41"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:N43"/>
@@ -21634,21 +21633,21 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="8" customWidth="1"/>
-    <col min="2" max="3" width="35.375" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="8" customWidth="1"/>
+    <col min="2" max="3" width="35.33203125" style="16" customWidth="1"/>
     <col min="4" max="5" width="33.5" style="157" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="193" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="10.625" style="193" customWidth="1"/>
+    <col min="7" max="10" width="10.6640625" style="193" customWidth="1"/>
     <col min="11" max="11" width="35" style="16" customWidth="1"/>
     <col min="12" max="12" width="15" style="16" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" style="16" customWidth="1"/>
-    <col min="14" max="14" width="26.875" style="16" customWidth="1"/>
-    <col min="15" max="16384" width="8.875" style="16"/>
+    <col min="14" max="14" width="26.83203125" style="16" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="47.25">
       <c r="A1" s="149" t="s">
         <v>286</v>
       </c>
@@ -21692,7 +21691,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="31.5">
       <c r="A2" s="151">
         <v>1</v>
       </c>
@@ -21736,7 +21735,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="151">
         <v>2</v>
       </c>
@@ -21778,7 +21777,7 @@
       </c>
       <c r="N3" s="19"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="151">
         <v>3</v>
       </c>
@@ -21822,7 +21821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="151">
         <v>4</v>
       </c>
@@ -21866,7 +21865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="151">
         <v>5</v>
       </c>
@@ -21910,7 +21909,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="151">
         <v>6</v>
       </c>
@@ -21952,7 +21951,7 @@
       </c>
       <c r="N7" s="19"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="151">
         <v>7</v>
       </c>
@@ -21994,7 +21993,7 @@
       </c>
       <c r="N8" s="19"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="151">
         <v>8</v>
       </c>
@@ -22036,7 +22035,7 @@
       </c>
       <c r="N9" s="19"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="151">
         <v>9</v>
       </c>
@@ -22078,7 +22077,7 @@
       </c>
       <c r="N10" s="19"/>
     </row>
-    <row r="11" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="31.5">
       <c r="A11" s="151">
         <v>10</v>
       </c>
@@ -22120,7 +22119,7 @@
       </c>
       <c r="N11" s="19"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="151">
         <v>11</v>
       </c>
@@ -22162,7 +22161,7 @@
       </c>
       <c r="N12" s="19"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="151">
         <v>12</v>
       </c>
@@ -22204,7 +22203,7 @@
       </c>
       <c r="N13" s="19"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" s="151">
         <v>13</v>
       </c>
@@ -22246,7 +22245,7 @@
       </c>
       <c r="N14" s="19"/>
     </row>
-    <row r="15" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="31.5">
       <c r="A15" s="151">
         <v>14</v>
       </c>
@@ -22288,7 +22287,7 @@
       </c>
       <c r="N15" s="19"/>
     </row>
-    <row r="16" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="31.5">
       <c r="A16" s="151">
         <v>15</v>
       </c>
@@ -22330,7 +22329,7 @@
       </c>
       <c r="N16" s="19"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" s="151">
         <v>16</v>
       </c>
@@ -22372,7 +22371,7 @@
       </c>
       <c r="N17" s="19"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" s="151">
         <v>17</v>
       </c>
@@ -22414,7 +22413,7 @@
       </c>
       <c r="N18" s="19"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" s="151">
         <v>18</v>
       </c>
@@ -22456,7 +22455,7 @@
       </c>
       <c r="N19" s="19"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="151">
         <v>19</v>
       </c>
@@ -22498,7 +22497,7 @@
       </c>
       <c r="N20" s="19"/>
     </row>
-    <row r="21" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="31.5">
       <c r="A21" s="151">
         <v>20</v>
       </c>
@@ -22540,7 +22539,7 @@
       </c>
       <c r="N21" s="19"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="151">
         <v>21</v>
       </c>
@@ -22582,7 +22581,7 @@
       </c>
       <c r="N22" s="19"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="151">
         <v>22</v>
       </c>
@@ -22624,7 +22623,7 @@
       </c>
       <c r="N23" s="19"/>
     </row>
-    <row r="24" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="31.5">
       <c r="A24" s="151">
         <v>23</v>
       </c>
@@ -22666,7 +22665,7 @@
       </c>
       <c r="N24" s="19"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="151">
         <v>24</v>
       </c>
@@ -22708,7 +22707,7 @@
       </c>
       <c r="N25" s="19"/>
     </row>
-    <row r="26" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="31.5">
       <c r="A26" s="151">
         <v>25</v>
       </c>
@@ -22750,7 +22749,7 @@
       </c>
       <c r="N26" s="19"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="151">
         <v>26</v>
       </c>
@@ -22792,7 +22791,7 @@
       </c>
       <c r="N27" s="19"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="151">
         <v>27</v>
       </c>
@@ -22834,7 +22833,7 @@
       </c>
       <c r="N28" s="19"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="151">
         <v>28</v>
       </c>
@@ -22876,7 +22875,7 @@
       </c>
       <c r="N29" s="19"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="151">
         <v>29</v>
       </c>
@@ -22918,7 +22917,7 @@
       </c>
       <c r="N30" s="19"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="151">
         <v>30</v>
       </c>
@@ -22960,7 +22959,7 @@
       </c>
       <c r="N31" s="19"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="151">
         <v>31</v>
       </c>
@@ -23002,7 +23001,7 @@
       </c>
       <c r="N32" s="19"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="151">
         <v>32</v>
       </c>
@@ -23044,7 +23043,7 @@
       </c>
       <c r="N33" s="19"/>
     </row>
-    <row r="34" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="31.5">
       <c r="A34" s="151">
         <v>33</v>
       </c>
@@ -23086,7 +23085,7 @@
       </c>
       <c r="N34" s="19"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" s="151">
         <v>34</v>
       </c>
@@ -23124,7 +23123,7 @@
       </c>
       <c r="N35" s="19"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="A36" s="151">
         <v>35</v>
       </c>
@@ -23162,7 +23161,7 @@
       </c>
       <c r="N36" s="19"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="A37" s="151">
         <v>36</v>
       </c>
@@ -23200,7 +23199,7 @@
       </c>
       <c r="N37" s="19"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" s="151">
         <v>37</v>
       </c>
@@ -23240,7 +23239,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="A39" s="151">
         <v>38</v>
       </c>
@@ -23280,7 +23279,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14">
       <c r="A40" s="151">
         <v>39</v>
       </c>
@@ -23320,7 +23319,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14">
       <c r="A41" s="151">
         <v>40</v>
       </c>
@@ -23358,7 +23357,7 @@
       </c>
       <c r="N41" s="19"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14">
       <c r="A42" s="151">
         <v>41</v>
       </c>
@@ -23400,7 +23399,7 @@
       </c>
       <c r="N42" s="19"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
@@ -23479,7 +23478,12 @@
     <hyperlink ref="K40" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="142" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId71"/>
-  <legacyDrawing r:id="rId72"/>
+  <pageSetup paperSize="142" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId71"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>